<commit_message>
Add Tests for Each Model Class
1) Finalize Issue tests
2) Create Collection tests
3) Create Series tests
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\git\SE2-project-repos-sample\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nginn1\Documents\GitHub\DevOps-Project-1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F82DD3F-9313-4318-A2E5-F07A5CD5C9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570B5C17-2685-4A2D-BF0E-1B5A4A59028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,15 +71,6 @@
     <t>Create a collection</t>
   </si>
   <si>
-    <t>Create an issue class</t>
-  </si>
-  <si>
-    <t>Create a series class that holds issue items</t>
-  </si>
-  <si>
-    <t>Create a collection class that holds series items</t>
-  </si>
-  <si>
     <t>Add a list box to view the users collections</t>
   </si>
   <si>
@@ -117,13 +108,22 @@
   </si>
   <si>
     <t>Estimate Totals</t>
+  </si>
+  <si>
+    <t>Create an issue class w/ tests</t>
+  </si>
+  <si>
+    <t>Create a series class that holds issue items w/ tests</t>
+  </si>
+  <si>
+    <t>Create a collection class that holds series items w/ tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,7 +325,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1379,17 +1379,17 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.42578125" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1423,7 +1423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1436,72 +1436,80 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="30.75">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1511,12 +1519,12 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="30.75">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1526,12 +1534,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1541,12 +1549,12 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="45.75">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1556,12 +1564,12 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="30.75">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1571,12 +1579,12 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -1586,12 +1594,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="30.75">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1601,12 +1609,12 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="30.75">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1616,7 +1624,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1625,7 +1633,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1634,7 +1642,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1643,7 +1651,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1652,7 +1660,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1661,7 +1669,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1670,7 +1678,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1679,7 +1687,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1688,7 +1696,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1697,7 +1705,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1706,10 +1714,10 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C26" s="3">
         <f>SUM(C3:C25)</f>
@@ -1717,7 +1725,7 @@
       </c>
       <c r="D26" s="3">
         <f t="shared" ref="D26:G26" si="0">SUM(D3:D25)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Create AddSeriesWindow, AddIssueWindow and ViewSeriesWindow
1) Created AddSeriesWindow.Java and AddSeriesWindow.fxml
2) Created AddIssueWindow.Java and AddIssueWindow.fxml
3) Created ViewSeriesWindow.Java and ViewSeriesWindow.fxml
4) Added functionality to MainWindow .java to open the AddSeriesWindow
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nginn1\Documents\GitHub\DevOps-Project-1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570B5C17-2685-4A2D-BF0E-1B5A4A59028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EBD653-8AA3-4927-9232-0D3E9658741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Related User Story</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Create a collection class that holds series items w/ tests</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1379,7 +1382,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,8 +1449,8 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1463,8 +1466,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1480,8 +1483,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1497,8 +1500,8 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1514,7 +1517,9 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1529,7 +1534,9 @@
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1544,7 +1551,9 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1559,7 +1568,9 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1574,7 +1585,9 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1725,7 +1738,7 @@
       </c>
       <c r="D26" s="3">
         <f t="shared" ref="D26:G26" si="0">SUM(D3:D25)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>

</xml_diff>